<commit_message>
Filtro de busqueda en la tabla equipos
Filtro de busqueda en la tabla equipos
</commit_message>
<xml_diff>
--- a/Documentos/Tabla Mejores Jugadores.xlsx
+++ b/Documentos/Tabla Mejores Jugadores.xlsx
@@ -6,13 +6,13 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Sheet1" sheetId="1" r:id="R39d5290f54bd4978"/>
+    <x:sheet name="Sheet1" sheetId="1" r:id="R3039eac40bfb4a20"/>
   </x:sheets>
 </x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <x:si>
     <x:t>Cantidad Votos</x:t>
   </x:si>
@@ -54,6 +54,9 @@
   </x:si>
   <x:si>
     <x:t>Fernandes</x:t>
+  </x:si>
+  <x:si>
+    <x:t>System.Byte[]</x:t>
   </x:si>
   <x:si>
     <x:t>Marcus</x:t>
@@ -458,7 +461,7 @@
     <x:col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
     <x:col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
     <x:col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
-    <x:col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
+    <x:col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
     <x:col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
     <x:col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
   </x:cols>
@@ -511,7 +514,9 @@
       <x:c r="C3" s="4" t="s">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="D3" s="3"/>
+      <x:c r="D3" s="4" t="s">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="E3" s="4" t="s">
         <x:v>9</x:v>
       </x:c>
@@ -524,10 +529,10 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="B4" s="4" t="s">
-        <x:v>14</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="C4" s="4" t="s">
-        <x:v>15</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="D4" s="3"/>
       <x:c r="E4" s="4" t="s">
@@ -542,10 +547,10 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="B5" s="4" t="s">
-        <x:v>16</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="C5" s="4" t="s">
-        <x:v>17</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="D5" s="3"/>
       <x:c r="E5" s="4" t="s">
@@ -560,28 +565,28 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="B6" s="4" t="s">
-        <x:v>18</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="C6" s="4" t="s">
-        <x:v>19</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="D6" s="3"/>
       <x:c r="E6" s="4" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="F6" s="4" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="7">
       <x:c r="A7" s="4" t="s">
-        <x:v>22</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="B7" s="4" t="s">
-        <x:v>23</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="C7" s="4" t="s">
-        <x:v>24</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="D7" s="3"/>
       <x:c r="E7" s="4" t="s">
@@ -593,20 +598,20 @@
     </x:row>
     <x:row r="8">
       <x:c r="A8" s="4" t="s">
-        <x:v>22</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="B8" s="4" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="C8" s="4" t="s">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="D8" s="3"/>
       <x:c r="E8" s="4" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="F8" s="4" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>